<commit_message>
changes to LISA P2
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_LISA_P2.xlsx
+++ b/rmonize/data_proc_elem/DPE_LISA_P2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C28429-97CF-430A-B239-424900291E3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D790FE3A-64EA-43A7-BE46-62096EBBCB9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22050" windowHeight="8280" xr2:uid="{786B4876-F99A-4BB7-BD43-A6CEAD3EC1AA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="328">
   <si>
     <t>Index</t>
   </si>
@@ -660,9 +660,6 @@
     <t>Fat mass index at baseline</t>
   </si>
   <si>
-    <t xml:space="preserve">UB_fmi_15 </t>
-  </si>
-  <si>
     <t>BODY_FAT_FUP</t>
   </si>
   <si>
@@ -868,9 +865,6 @@
   </si>
   <si>
     <t>Sodium to potassium intake ratio [g/d]</t>
-  </si>
-  <si>
-    <t>num</t>
   </si>
   <si>
     <t>FFQMK_15;
@@ -1106,6 +1100,9 @@
   </si>
   <si>
     <t>recode(1= 1; 2 = 3; 3=3; 4 = 3; 5=3)</t>
+  </si>
+  <si>
+    <t>UB_fmi_15</t>
   </si>
 </sst>
 </file>
@@ -1625,8 +1622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CB6D67-1D35-4768-BA1C-E9D0A324CEEE}">
   <dimension ref="A1:L131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1801,7 +1798,7 @@
         <v>28</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>29</v>
@@ -1836,7 +1833,7 @@
         <v>28</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>34</v>
@@ -1970,7 +1967,7 @@
         <v>52</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>35</v>
@@ -2524,7 +2521,7 @@
         <v>52</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>16</v>
@@ -2586,7 +2583,7 @@
         <v>28</v>
       </c>
       <c r="H29" s="26" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="I29" s="25" t="s">
         <v>105</v>
@@ -3772,7 +3769,9 @@
       <c r="G66" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H66" s="2"/>
+      <c r="H66" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="I66" s="2"/>
       <c r="J66" s="2" t="s">
         <v>16</v>
@@ -3803,7 +3802,9 @@
       <c r="G67" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H67" s="2"/>
+      <c r="H67" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="I67" s="2"/>
       <c r="J67" s="2" t="s">
         <v>16</v>
@@ -3832,7 +3833,9 @@
       <c r="G68" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H68" s="2"/>
+      <c r="H68" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="I68" s="2"/>
       <c r="J68" s="2" t="s">
         <v>16</v>
@@ -3890,7 +3893,9 @@
       <c r="G70" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H70" s="2"/>
+      <c r="H70" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="I70" s="2"/>
       <c r="J70" s="2" t="s">
         <v>39</v>
@@ -3917,7 +3922,9 @@
       <c r="G71" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H71" s="2"/>
+      <c r="H71" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="I71" s="2"/>
       <c r="J71" s="2" t="s">
         <v>39</v>
@@ -3944,7 +3951,9 @@
       <c r="G72" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H72" s="2"/>
+      <c r="H72" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="I72" s="2"/>
       <c r="J72" s="2" t="s">
         <v>39</v>
@@ -3971,7 +3980,9 @@
       <c r="G73" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H73" s="2"/>
+      <c r="H73" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="I73" s="2"/>
       <c r="J73" s="2" t="s">
         <v>39</v>
@@ -4000,7 +4011,9 @@
       <c r="G74" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H74" s="2"/>
+      <c r="H74" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="I74" s="2"/>
       <c r="J74" s="2" t="s">
         <v>39</v>
@@ -4026,12 +4039,14 @@
         <v>14</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>203</v>
+        <v>327</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H75" s="2"/>
+      <c r="H75" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="I75" s="2"/>
       <c r="J75" s="2" t="s">
         <v>16</v>
@@ -4045,10 +4060,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="2" t="s">
@@ -4058,7 +4073,9 @@
       <c r="G76" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H76" s="2"/>
+      <c r="H76" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="I76" s="2"/>
       <c r="J76" s="2" t="s">
         <v>39</v>
@@ -4072,10 +4089,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>80</v>
@@ -4084,14 +4101,16 @@
         <v>14</v>
       </c>
       <c r="F77" s="24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H77" s="2"/>
+      <c r="H77" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="I77" s="24" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J77" s="2" t="s">
         <v>16</v>
@@ -4105,10 +4124,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>80</v>
@@ -4117,12 +4136,14 @@
         <v>14</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H78" s="2"/>
+      <c r="H78" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="I78" s="2"/>
       <c r="J78" s="2" t="s">
         <v>16</v>
@@ -4136,10 +4157,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C79" s="15" t="s">
         <v>213</v>
-      </c>
-      <c r="C79" s="15" t="s">
-        <v>214</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>80</v>
@@ -4148,12 +4169,14 @@
         <v>14</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H79" s="2"/>
+      <c r="H79" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="I79" s="2"/>
       <c r="J79" s="2" t="s">
         <v>16</v>
@@ -4167,10 +4190,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C80" s="15" t="s">
         <v>216</v>
-      </c>
-      <c r="C80" s="15" t="s">
-        <v>217</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>80</v>
@@ -4179,13 +4202,13 @@
         <v>14</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I80" s="2"/>
       <c r="J80" s="2" t="s">
@@ -4200,10 +4223,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C81" s="15" t="s">
         <v>220</v>
-      </c>
-      <c r="C81" s="15" t="s">
-        <v>221</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>80</v>
@@ -4212,13 +4235,13 @@
         <v>14</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I81" s="2"/>
       <c r="J81" s="2" t="s">
@@ -4233,10 +4256,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C82" s="15" t="s">
         <v>224</v>
-      </c>
-      <c r="C82" s="15" t="s">
-        <v>225</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>80</v>
@@ -4245,13 +4268,13 @@
         <v>14</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I82" s="2"/>
       <c r="J82" s="2" t="s">
@@ -4266,10 +4289,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C83" s="15" t="s">
         <v>228</v>
-      </c>
-      <c r="C83" s="15" t="s">
-        <v>229</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>80</v>
@@ -4278,13 +4301,13 @@
         <v>14</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I83" s="2"/>
       <c r="J83" s="2" t="s">
@@ -4299,10 +4322,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C84" s="15" t="s">
         <v>232</v>
-      </c>
-      <c r="C84" s="15" t="s">
-        <v>233</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>80</v>
@@ -4311,13 +4334,13 @@
         <v>14</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I84" s="2"/>
       <c r="J84" s="2" t="s">
@@ -4332,10 +4355,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C85" s="15" t="s">
         <v>236</v>
-      </c>
-      <c r="C85" s="15" t="s">
-        <v>237</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>80</v>
@@ -4344,13 +4367,13 @@
         <v>14</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I85" s="2"/>
       <c r="J85" s="2" t="s">
@@ -4365,10 +4388,10 @@
         <v>85</v>
       </c>
       <c r="B86" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C86" s="15" t="s">
         <v>240</v>
-      </c>
-      <c r="C86" s="15" t="s">
-        <v>241</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>80</v>
@@ -4377,13 +4400,13 @@
         <v>14</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I86" s="2"/>
       <c r="J86" s="2" t="s">
@@ -4398,10 +4421,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C87" s="15" t="s">
         <v>244</v>
-      </c>
-      <c r="C87" s="15" t="s">
-        <v>245</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>80</v>
@@ -4410,13 +4433,13 @@
         <v>14</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G87" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I87" s="2"/>
       <c r="J87" s="2" t="s">
@@ -4431,10 +4454,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C88" s="15" t="s">
         <v>248</v>
-      </c>
-      <c r="C88" s="15" t="s">
-        <v>249</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>80</v>
@@ -4446,7 +4469,9 @@
       <c r="G88" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H88" s="2"/>
+      <c r="H88" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="I88" s="2"/>
       <c r="J88" s="2" t="s">
         <v>39</v>
@@ -4460,10 +4485,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C89" s="15" t="s">
         <v>250</v>
-      </c>
-      <c r="C89" s="15" t="s">
-        <v>251</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>80</v>
@@ -4475,7 +4500,9 @@
       <c r="G89" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H89" s="2"/>
+      <c r="H89" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="I89" s="2"/>
       <c r="J89" s="2" t="s">
         <v>39</v>
@@ -4489,10 +4516,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C90" s="15" t="s">
         <v>252</v>
-      </c>
-      <c r="C90" s="15" t="s">
-        <v>253</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>80</v>
@@ -4504,7 +4531,9 @@
       <c r="G90" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H90" s="2"/>
+      <c r="H90" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="I90" s="2"/>
       <c r="J90" s="2" t="s">
         <v>39</v>
@@ -4518,10 +4547,10 @@
         <v>90</v>
       </c>
       <c r="B91" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C91" s="15" t="s">
         <v>254</v>
-      </c>
-      <c r="C91" s="15" t="s">
-        <v>255</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>80</v>
@@ -4530,13 +4559,13 @@
         <v>14</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I91" s="2"/>
       <c r="J91" s="2" t="s">
@@ -4551,10 +4580,10 @@
         <v>91</v>
       </c>
       <c r="B92" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C92" s="15" t="s">
         <v>258</v>
-      </c>
-      <c r="C92" s="15" t="s">
-        <v>259</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>80</v>
@@ -4563,13 +4592,13 @@
         <v>14</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I92" s="2"/>
       <c r="J92" s="2" t="s">
@@ -4584,10 +4613,10 @@
         <v>92</v>
       </c>
       <c r="B93" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>263</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>80</v>
@@ -4596,16 +4625,16 @@
         <v>14</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>264</v>
+        <v>21</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J93" s="2" t="s">
         <v>16</v>
@@ -4619,10 +4648,10 @@
         <v>93</v>
       </c>
       <c r="B94" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>266</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>80</v>
@@ -4631,16 +4660,16 @@
         <v>14</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>264</v>
+        <v>21</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J94" s="2" t="s">
         <v>16</v>
@@ -4654,10 +4683,10 @@
         <v>94</v>
       </c>
       <c r="B95" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C95" s="15" t="s">
         <v>267</v>
-      </c>
-      <c r="C95" s="15" t="s">
-        <v>268</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>80</v>
@@ -4666,13 +4695,13 @@
         <v>14</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G95" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I95" s="2"/>
       <c r="J95" s="2" t="s">
@@ -4687,25 +4716,25 @@
         <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C96" s="15" t="s">
         <v>271</v>
       </c>
-      <c r="C96" s="15" t="s">
+      <c r="D96" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F96" s="3" t="s">
         <v>272</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F96" s="3" t="s">
-        <v>274</v>
       </c>
       <c r="G96" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I96" s="2"/>
       <c r="J96" s="2" t="s">
@@ -4720,25 +4749,25 @@
         <v>96</v>
       </c>
       <c r="B97" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C97" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F97" s="3" t="s">
         <v>276</v>
-      </c>
-      <c r="C97" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F97" s="3" t="s">
-        <v>278</v>
       </c>
       <c r="G97" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I97" s="2"/>
       <c r="J97" s="2" t="s">
@@ -4753,25 +4782,25 @@
         <v>97</v>
       </c>
       <c r="B98" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C98" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F98" s="3" t="s">
         <v>280</v>
-      </c>
-      <c r="C98" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F98" s="3" t="s">
-        <v>282</v>
       </c>
       <c r="G98" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H98" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I98" s="2"/>
       <c r="J98" s="2" t="s">
@@ -4786,25 +4815,25 @@
         <v>98</v>
       </c>
       <c r="B99" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C99" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F99" s="3" t="s">
         <v>284</v>
-      </c>
-      <c r="C99" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F99" s="3" t="s">
-        <v>286</v>
       </c>
       <c r="G99" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I99" s="2"/>
       <c r="J99" s="2" t="s">
@@ -4819,25 +4848,25 @@
         <v>99</v>
       </c>
       <c r="B100" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C100" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F100" s="3" t="s">
         <v>288</v>
-      </c>
-      <c r="C100" s="17" t="s">
-        <v>289</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F100" s="3" t="s">
-        <v>290</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="I100" s="2"/>
       <c r="J100" s="2" t="s">
@@ -4852,13 +4881,13 @@
         <v>100</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C101" s="17" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>273</v>
+        <v>80</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>14</v>
@@ -4867,7 +4896,9 @@
       <c r="G101" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H101" s="2"/>
+      <c r="H101" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="I101" s="2"/>
       <c r="J101" s="2" t="s">
         <v>39</v>
@@ -4881,25 +4912,25 @@
         <v>101</v>
       </c>
       <c r="B102" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C102" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F102" s="3" t="s">
         <v>294</v>
-      </c>
-      <c r="C102" s="17" t="s">
-        <v>295</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E102" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F102" s="3" t="s">
-        <v>296</v>
       </c>
       <c r="G102" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I102" s="2"/>
       <c r="J102" s="2" t="s">
@@ -4914,14 +4945,12 @@
         <v>102</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C103" s="15" t="s">
-        <v>299</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>273</v>
-      </c>
+        <v>297</v>
+      </c>
+      <c r="D103" s="2"/>
       <c r="E103" s="2" t="s">
         <v>14</v>
       </c>
@@ -4929,7 +4958,9 @@
       <c r="G103" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H103" s="2"/>
+      <c r="H103" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="I103" s="2"/>
       <c r="J103" s="2" t="s">
         <v>39</v>
@@ -4943,25 +4974,25 @@
         <v>103</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C104" s="16" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>273</v>
+        <v>80</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="G104" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="I104" s="2"/>
       <c r="J104" s="2" t="s">
@@ -4976,25 +5007,25 @@
         <v>104</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C105" s="17" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>273</v>
+        <v>80</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G105" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="I105" s="2"/>
       <c r="J105" s="2" t="s">
@@ -5009,25 +5040,25 @@
         <v>105</v>
       </c>
       <c r="B106" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C106" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F106" s="3" t="s">
         <v>304</v>
-      </c>
-      <c r="C106" s="17" t="s">
-        <v>305</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E106" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F106" s="3" t="s">
-        <v>306</v>
       </c>
       <c r="G106" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I106" s="2"/>
       <c r="J106" s="2" t="s">
@@ -5042,13 +5073,13 @@
         <v>106</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C107" s="17" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>273</v>
+        <v>80</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>14</v>
@@ -5057,7 +5088,9 @@
       <c r="G107" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H107" s="2"/>
+      <c r="H107" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="I107" s="2"/>
       <c r="J107" s="2" t="s">
         <v>39</v>
@@ -5071,24 +5104,26 @@
         <v>107</v>
       </c>
       <c r="B108" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C108" s="17" t="s">
+        <v>309</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F108" s="2" t="s">
         <v>310</v>
-      </c>
-      <c r="C108" s="17" t="s">
-        <v>311</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F108" s="2" t="s">
-        <v>312</v>
       </c>
       <c r="G108" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H108" s="2"/>
+      <c r="H108" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="I108" s="2"/>
       <c r="J108" s="2" t="s">
         <v>16</v>
@@ -5102,28 +5137,28 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
+        <v>311</v>
+      </c>
+      <c r="C109" t="s">
+        <v>312</v>
+      </c>
+      <c r="D109" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="E109" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F109" s="30" t="s">
         <v>313</v>
       </c>
-      <c r="C109" t="s">
+      <c r="G109" s="31" t="s">
         <v>314</v>
-      </c>
-      <c r="D109" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="E109" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="F109" s="30" t="s">
-        <v>315</v>
-      </c>
-      <c r="G109" s="31" t="s">
-        <v>316</v>
       </c>
       <c r="H109">
         <v>1</v>
       </c>
       <c r="I109" s="32" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="J109" s="15" t="s">
         <v>16</v>
@@ -5206,6 +5241,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -5446,18 +5493,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5468,6 +5503,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B65EFA2E-A807-485E-9383-5A8846A1595A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B924E26-FD9D-4578-A9DC-389C0AAF7136}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5486,17 +5532,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B65EFA2E-A807-485E-9383-5A8846A1595A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07CD54F7-7682-4260-A57C-9131D22DC2E8}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
DPE LISA P2 small change in dietary instrument comment
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_LISA_P2.xlsx
+++ b/rmonize/data_proc_elem/DPE_LISA_P2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B210221-F2A7-4589-AC23-A8D6AF29A173}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2A6D52-CFE2-45E4-9CBE-C1CFDD0A8995}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22050" windowHeight="8280" xr2:uid="{786B4876-F99A-4BB7-BD43-A6CEAD3EC1AA}"/>
   </bookViews>
@@ -924,9 +924,6 @@
     <t>paste</t>
   </si>
   <si>
-    <t>FFQs</t>
-  </si>
-  <si>
     <t>FFQAPFEL_15;
 FFQBEERE_15;
 FFQSUED_15;
@@ -1106,6 +1103,9 @@
   </si>
   <si>
     <t>Total fruit intake [g/d]</t>
+  </si>
+  <si>
+    <t>1 (FFQ)</t>
   </si>
 </sst>
 </file>
@@ -1606,8 +1606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CB6D67-1D35-4768-BA1C-E9D0A324CEEE}">
   <dimension ref="A1:L131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D109"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I112" sqref="I112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1734,7 +1734,7 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D4" t="s">
         <v>70</v>
@@ -1782,7 +1782,7 @@
         <v>27</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>28</v>
@@ -1817,7 +1817,7 @@
         <v>27</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>33</v>
@@ -1869,7 +1869,7 @@
         <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D8" t="s">
         <v>70</v>
@@ -1904,7 +1904,7 @@
         <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D9" t="s">
         <v>70</v>
@@ -1951,7 +1951,7 @@
         <v>49</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>34</v>
@@ -1968,7 +1968,7 @@
         <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D11" t="s">
         <v>70</v>
@@ -2000,7 +2000,7 @@
         <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D12" t="s">
         <v>70</v>
@@ -2032,7 +2032,7 @@
         <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D13" t="s">
         <v>70</v>
@@ -2165,7 +2165,7 @@
         <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
@@ -2198,7 +2198,7 @@
         <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D18" t="s">
         <v>13</v>
@@ -2230,7 +2230,7 @@
         <v>68</v>
       </c>
       <c r="C19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D19" t="s">
         <v>70</v>
@@ -2262,7 +2262,7 @@
         <v>69</v>
       </c>
       <c r="C20" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D20" t="s">
         <v>70</v>
@@ -2295,7 +2295,7 @@
         <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D21" t="s">
         <v>70</v>
@@ -2328,7 +2328,7 @@
         <v>74</v>
       </c>
       <c r="C22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D22" t="s">
         <v>70</v>
@@ -2361,7 +2361,7 @@
         <v>76</v>
       </c>
       <c r="C23" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D23" t="s">
         <v>70</v>
@@ -2505,7 +2505,7 @@
         <v>49</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>16</v>
@@ -2567,7 +2567,7 @@
         <v>27</v>
       </c>
       <c r="H29" s="21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I29" s="20" t="s">
         <v>92</v>
@@ -2747,7 +2747,7 @@
         <v>103</v>
       </c>
       <c r="C35" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D35" t="s">
         <v>13</v>
@@ -2779,7 +2779,7 @@
         <v>104</v>
       </c>
       <c r="C36" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D36" t="s">
         <v>13</v>
@@ -2811,7 +2811,7 @@
         <v>105</v>
       </c>
       <c r="C37" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D37" t="s">
         <v>13</v>
@@ -3516,10 +3516,10 @@
         <v>148</v>
       </c>
       <c r="C59" t="s">
+        <v>306</v>
+      </c>
+      <c r="D59" t="s">
         <v>307</v>
-      </c>
-      <c r="D59" t="s">
-        <v>308</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>14</v>
@@ -3707,7 +3707,7 @@
         <v>160</v>
       </c>
       <c r="C65" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D65" t="s">
         <v>70</v>
@@ -3739,7 +3739,7 @@
         <v>161</v>
       </c>
       <c r="C66" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D66" t="s">
         <v>70</v>
@@ -3772,7 +3772,7 @@
         <v>163</v>
       </c>
       <c r="C67" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D67" t="s">
         <v>70</v>
@@ -3805,7 +3805,7 @@
         <v>165</v>
       </c>
       <c r="C68" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -3838,7 +3838,7 @@
         <v>167</v>
       </c>
       <c r="C69" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D69" t="s">
         <v>70</v>
@@ -3871,7 +3871,7 @@
         <v>169</v>
       </c>
       <c r="C70" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D70" t="s">
         <v>70</v>
@@ -3902,7 +3902,7 @@
         <v>170</v>
       </c>
       <c r="C71" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D71" t="s">
         <v>70</v>
@@ -3933,7 +3933,7 @@
         <v>171</v>
       </c>
       <c r="C72" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D72" t="s">
         <v>70</v>
@@ -3964,7 +3964,7 @@
         <v>172</v>
       </c>
       <c r="C73" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D73" t="s">
         <v>70</v>
@@ -3995,7 +3995,7 @@
         <v>173</v>
       </c>
       <c r="C74" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D74" t="s">
         <v>70</v>
@@ -4026,7 +4026,7 @@
         <v>174</v>
       </c>
       <c r="C75" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D75" t="s">
         <v>70</v>
@@ -4035,7 +4035,7 @@
         <v>14</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>21</v>
@@ -4059,7 +4059,7 @@
         <v>175</v>
       </c>
       <c r="C76" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D76" t="s">
         <v>70</v>
@@ -4090,7 +4090,7 @@
         <v>176</v>
       </c>
       <c r="C77" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D77" t="s">
         <v>70</v>
@@ -4125,7 +4125,7 @@
         <v>179</v>
       </c>
       <c r="C78" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D78" t="s">
         <v>70</v>
@@ -4623,7 +4623,7 @@
         <v>14</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>21</v>
@@ -4649,7 +4649,7 @@
         <v>233</v>
       </c>
       <c r="C94" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D94" t="s">
         <v>70</v>
@@ -4658,7 +4658,7 @@
         <v>14</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>21</v>
@@ -4783,7 +4783,7 @@
         <v>246</v>
       </c>
       <c r="C98" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D98" t="s">
         <v>70</v>
@@ -4816,7 +4816,7 @@
         <v>249</v>
       </c>
       <c r="C99" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D99" t="s">
         <v>70</v>
@@ -4849,7 +4849,7 @@
         <v>252</v>
       </c>
       <c r="C100" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D100" t="s">
         <v>70</v>
@@ -4946,7 +4946,7 @@
         <v>261</v>
       </c>
       <c r="C103" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D103" t="s">
         <v>70</v>
@@ -4977,7 +4977,7 @@
         <v>262</v>
       </c>
       <c r="C104" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D104" t="s">
         <v>70</v>
@@ -4986,13 +4986,13 @@
         <v>14</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G104" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I104" s="2"/>
       <c r="J104" s="2" t="s">
@@ -5019,13 +5019,13 @@
         <v>14</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G105" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I105" s="2"/>
       <c r="J105" s="2" t="s">
@@ -5158,7 +5158,7 @@
         <v>1</v>
       </c>
       <c r="I109" s="27" t="s">
-        <v>278</v>
+        <v>328</v>
       </c>
       <c r="J109" s="11" t="s">
         <v>16</v>
@@ -5241,12 +5241,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5491,21 +5494,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07CD54F7-7682-4260-A57C-9131D22DC2E8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B65EFA2E-A807-485E-9383-5A8846A1595A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5530,12 +5533,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B65EFA2E-A807-485E-9383-5A8846A1595A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07CD54F7-7682-4260-A57C-9131D22DC2E8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GL-4 DPE_LISA_P2 updated algorithm for FAM1_DIAB2
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_LISA_P2.xlsx
+++ b/rmonize/data_proc_elem/DPE_LISA_P2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6597F160-F8D0-4600-B5E0-B280F806E304}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749071AA-6074-4F62-A214-996C4D63BBF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22050" windowHeight="8280" xr2:uid="{786B4876-F99A-4BB7-BD43-A6CEAD3EC1AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="22290" windowHeight="12000" xr2:uid="{786B4876-F99A-4BB7-BD43-A6CEAD3EC1AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1083,11 +1083,6 @@
     <t>Age at time of death [years]</t>
   </si>
   <si>
-    <t xml:space="preserve">If either parent has diabetes, the family history is marked as 1.
-If both parents do not have diabetes, the family history is marked as 0.                                                                                         If one parent's status is no or unknown (NA or 3), the family history is marked as 2. 
-If one parent's status is missing or unknown (NA or 3), the family history is marked as 2. </t>
-  </si>
-  <si>
     <t>Sodium intake [mg/d]</t>
   </si>
   <si>
@@ -1095,13 +1090,17 @@
   </si>
   <si>
     <t>case_when (
-  diabmut_15 == 1 | diabvat_15 == 1 ~ 1L,
-  diabmut_15 == 0 &amp; diabvat_15 == 0 ~ 0L,
-   diabmut_15 == 3 &amp; diabvat_15 == 0 ~ 2L,
-  diabvat_15 == 3 &amp; diabmut_15 == 0 ~ 2L,
-  (is.na(diabmut_15)  &amp;  diabvat_15 == 3 ~ 2L,  (is.na(diabvat_15)  &amp;  diabmut_15 == 3 ~ 2L, 
-  TRUE ~ NA_integer_
+      diabmut_15 == 1 | diabvat_15 == 1 ~ 1L,
+      diabmut_15 == 3 | diabvat_15 == 3 ~ 2L,
+      diabmut_15 == 2 &amp; diabvat_15 == 2 ~ 0L,
+      TRUE ~ NA_integer_
 )</t>
+  </si>
+  <si>
+    <t>If either parent has diabetes(1), the family history is marked as yes(1).
+If one parent's status is unknown (3), the family history is marked as don't know (2). 
+If both parents do not have diabetes (2), the family history is marked as no (0).
+Everything else (e.g. 2+ NA, NA+NA) is marked as NA</t>
   </si>
 </sst>
 </file>
@@ -1304,9 +1303,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1344,7 +1343,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1450,7 +1449,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1592,7 +1591,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1602,8 +1601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CB6D67-1D35-4768-BA1C-E9D0A324CEEE}">
   <dimension ref="A1:L131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I94" sqref="I94"/>
+    <sheetView tabSelected="1" topLeftCell="F12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2540,7 +2539,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="1" customFormat="1" ht="135">
+    <row r="29" spans="1:11" s="1" customFormat="1" ht="105">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2563,10 +2562,10 @@
         <v>27</v>
       </c>
       <c r="H29" s="21" t="s">
+        <v>326</v>
+      </c>
+      <c r="I29" s="20" t="s">
         <v>327</v>
-      </c>
-      <c r="I29" s="20" t="s">
-        <v>324</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>34</v>
@@ -4680,7 +4679,7 @@
         <v>222</v>
       </c>
       <c r="C95" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D95" t="s">
         <v>70</v>
@@ -4713,7 +4712,7 @@
         <v>224</v>
       </c>
       <c r="C96" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D96" t="s">
         <v>70</v>
@@ -5237,12 +5236,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5487,21 +5489,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07CD54F7-7682-4260-A57C-9131D22DC2E8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B65EFA2E-A807-485E-9383-5A8846A1595A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5526,12 +5528,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B65EFA2E-A807-485E-9383-5A8846A1595A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07CD54F7-7682-4260-A57C-9131D22DC2E8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GL-4 DPE_LISA_P2 updated EDU_LEVEL and FAM_DIAB2
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_LISA_P2.xlsx
+++ b/rmonize/data_proc_elem/DPE_LISA_P2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749071AA-6074-4F62-A214-996C4D63BBF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A46C7C-B15D-4E93-BE5E-5A76A8DDA32A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="22290" windowHeight="12000" xr2:uid="{786B4876-F99A-4BB7-BD43-A6CEAD3EC1AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="22260" windowHeight="12000" xr2:uid="{786B4876-F99A-4BB7-BD43-A6CEAD3EC1AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,14 +112,6 @@
     <t>case_when</t>
   </si>
   <si>
-    <t>"None" (0): Both parents have 1 (no certificate).
-"Primary School Completed" (1): Either parent has 2.
-"Technical/Professional School" (2): Either parent has 3.
-"Secondary School" (3): Either parent has 4.
-"Longer Education" (4): Either parent has 5 or 6.
-"Not Specified" (5): Either parent has 7 (other degree).</t>
-  </si>
-  <si>
     <t>compatible</t>
   </si>
   <si>
@@ -894,17 +886,6 @@
   <si>
     <t>FFQRIND_15 +
 FFQSCHW_15</t>
-  </si>
-  <si>
-    <t>case_when(
-      MUTBILD_0 == 1 &amp; VATBILD_0 == 1 ~ 0L,
-      MUTBILD_0 %in% c(2) | VATBILD_0 %in% c(2) ~ 1L,  
-      MUTBILD_0 %in% c(3) | VATBILD_0 %in% c(3) ~ 2L, 
-      MUTBILD_0 %in% c(4) | VATBILD_0 %in% c(4) ~ 3L, 
-      MUTBILD_0 %in% c(5, 6) | VATBILD_0 %in% c(5, 6) ~ 4L, 
-      MUTBILD_0 %in% c(7) | VATBILD_0 %in% c(7) ~ 5L,  
-      TRUE ~ NA_integer_
-    )</t>
   </si>
   <si>
     <t>case_when(
@@ -1089,18 +1070,37 @@
     <t>Sodium to potassium intake ratio</t>
   </si>
   <si>
+    <t>case_when(
+      MUTBILD_0 == 1 &amp; VATBILD_0 == 1 ~ 0L,
+      MUTBILD_0 %in% c(2) | VATBILD_0 %in% c(2) ~ 1L,  
+      MUTBILD_0 %in% c(3) | VATBILD_0 %in% c(3) ~ 3L, 
+      MUTBILD_0 %in% c(4) | VATBILD_0 %in% c(4) ~ 2L, 
+      MUTBILD_0 %in% c(5, 6) | VATBILD_0 %in% c(5, 6) ~ 4L, 
+      MUTBILD_0 %in% c(7) | VATBILD_0 %in% c(7) ~ 5L,  
+      TRUE ~ NA_integer_
+    )</t>
+  </si>
+  <si>
+    <t>"None" (0): Both parents have 1 (no certificate).
+"Primary School Completed" (1): Either parent has 2.
+"Technical/Professional School" (2): Either parent has 4.
+"Secondary School" (3): Either parent has 3.
+"Longer Education" (4): Either parent has 5 or 6.
+"Not Specified" (5): Either parent has 7 (other degree).</t>
+  </si>
+  <si>
     <t>case_when (
       diabmut_15 == 1 | diabvat_15 == 1 ~ 1L,
+      diabmut_15 == 2 | diabvat_15 == 2 ~ 0L,
       diabmut_15 == 3 | diabvat_15 == 3 ~ 2L,
-      diabmut_15 == 2 &amp; diabvat_15 == 2 ~ 0L,
       TRUE ~ NA_integer_
 )</t>
   </si>
   <si>
-    <t>If either parent has diabetes(1), the family history is marked as yes(1).
-If one parent's status is unknown (3), the family history is marked as don't know (2). 
-If both parents do not have diabetes (2), the family history is marked as no (0).
-Everything else (e.g. 2+ NA, NA+NA) is marked as NA</t>
+    <t>If either parent has diabetes (coded as 1), the family history is marked as Yes (1).
+If both parents do not have diabetes (coded as 2), and condition 1 does not apply, the family history is marked as No (0).
+If either parent's diabetes status is unknown (coded as 3), and conditions 1 and 2 do not apply, the family history is marked as Don't Know (2).
+All other cases are marked as NA.</t>
   </si>
 </sst>
 </file>
@@ -1601,8 +1601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CB6D67-1D35-4768-BA1C-E9D0A324CEEE}">
   <dimension ref="A1:L131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="F21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1611,7 +1611,7 @@
     <col min="3" max="3" width="25.85546875" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.42578125" customWidth="1"/>
-    <col min="8" max="8" width="46" customWidth="1"/>
+    <col min="8" max="8" width="52.42578125" customWidth="1"/>
     <col min="9" max="9" width="54.28515625" customWidth="1"/>
     <col min="10" max="10" width="20.85546875" customWidth="1"/>
     <col min="11" max="11" width="18.42578125" customWidth="1"/>
@@ -1729,10 +1729,10 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
@@ -1751,10 +1751,10 @@
         <v>16</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="210">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="135">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1777,27 +1777,27 @@
         <v>27</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>267</v>
+        <v>324</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>28</v>
+        <v>325</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" ht="225">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="1" customFormat="1" ht="150">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
         <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -1806,22 +1806,22 @@
         <v>14</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="I6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1829,10 +1829,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
         <v>36</v>
-      </c>
-      <c r="C7" t="s">
-        <v>37</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -1841,54 +1841,54 @@
         <v>14</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" ht="105">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="1" customFormat="1" ht="90">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>271</v>
+      </c>
+      <c r="D8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C8" t="s">
-        <v>273</v>
-      </c>
-      <c r="D8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="23" t="s">
+      <c r="G8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="I8" s="19" t="s">
         <v>43</v>
-      </c>
-      <c r="I8" s="19" t="s">
-        <v>44</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1">
@@ -1896,31 +1896,31 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1">
@@ -1928,10 +1928,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
         <v>46</v>
-      </c>
-      <c r="C10" t="s">
-        <v>47</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -1940,19 +1940,19 @@
         <v>14</v>
       </c>
       <c r="F10" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="H10" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="J10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1960,31 +1960,31 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1992,31 +1992,31 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -2024,31 +2024,31 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -2056,10 +2056,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
         <v>53</v>
-      </c>
-      <c r="C14" t="s">
-        <v>54</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
@@ -2068,22 +2068,22 @@
         <v>14</v>
       </c>
       <c r="F14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H14" s="5" t="s">
+      <c r="I14" t="s">
         <v>56</v>
-      </c>
-      <c r="I14" t="s">
-        <v>57</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1">
@@ -2091,10 +2091,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" t="s">
         <v>58</v>
-      </c>
-      <c r="C15" t="s">
-        <v>59</v>
       </c>
       <c r="D15" t="s">
         <v>13</v>
@@ -2104,19 +2104,19 @@
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I15" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:12" s="1" customFormat="1">
@@ -2124,10 +2124,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" t="s">
         <v>62</v>
-      </c>
-      <c r="C16" t="s">
-        <v>63</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
@@ -2137,19 +2137,19 @@
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="1" customFormat="1">
@@ -2157,10 +2157,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
@@ -2170,19 +2170,19 @@
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="1" customFormat="1">
@@ -2190,10 +2190,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D18" t="s">
         <v>13</v>
@@ -2202,19 +2202,19 @@
         <v>14</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -2222,31 +2222,31 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -2254,19 +2254,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C20" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>21</v>
@@ -2279,7 +2279,7 @@
         <v>16</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -2287,19 +2287,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" t="s">
+        <v>280</v>
+      </c>
+      <c r="D21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="C21" t="s">
-        <v>282</v>
-      </c>
-      <c r="D21" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>21</v>
@@ -2312,7 +2312,7 @@
         <v>16</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -2320,19 +2320,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" t="s">
+        <v>281</v>
+      </c>
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="C22" t="s">
-        <v>283</v>
-      </c>
-      <c r="D22" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>21</v>
@@ -2345,7 +2345,7 @@
         <v>16</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -2353,19 +2353,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" t="s">
+        <v>282</v>
+      </c>
+      <c r="D23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="C23" t="s">
-        <v>284</v>
-      </c>
-      <c r="D23" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>21</v>
@@ -2378,7 +2378,7 @@
         <v>16</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -2386,10 +2386,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" t="s">
         <v>78</v>
-      </c>
-      <c r="C24" t="s">
-        <v>79</v>
       </c>
       <c r="D24" t="s">
         <v>13</v>
@@ -2398,19 +2398,19 @@
         <v>14</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -2418,10 +2418,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" t="s">
         <v>80</v>
-      </c>
-      <c r="C25" t="s">
-        <v>81</v>
       </c>
       <c r="D25" t="s">
         <v>13</v>
@@ -2430,19 +2430,19 @@
         <v>14</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -2450,10 +2450,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" t="s">
         <v>82</v>
-      </c>
-      <c r="C26" t="s">
-        <v>83</v>
       </c>
       <c r="D26" t="s">
         <v>13</v>
@@ -2462,19 +2462,19 @@
         <v>14</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="1" customFormat="1">
@@ -2482,10 +2482,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" t="s">
         <v>84</v>
-      </c>
-      <c r="C27" t="s">
-        <v>85</v>
       </c>
       <c r="D27" t="s">
         <v>13</v>
@@ -2494,19 +2494,19 @@
         <v>14</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>16</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="1" customFormat="1">
@@ -2514,10 +2514,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" t="s">
         <v>87</v>
-      </c>
-      <c r="C28" t="s">
-        <v>88</v>
       </c>
       <c r="D28" t="s">
         <v>13</v>
@@ -2527,27 +2527,27 @@
       </c>
       <c r="F28" s="16"/>
       <c r="G28" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J28" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" s="1" customFormat="1" ht="105">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="1" customFormat="1" ht="135">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" t="s">
         <v>89</v>
-      </c>
-      <c r="C29" t="s">
-        <v>90</v>
       </c>
       <c r="D29" t="s">
         <v>13</v>
@@ -2556,7 +2556,7 @@
         <v>14</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G29" s="22" t="s">
         <v>27</v>
@@ -2568,10 +2568,10 @@
         <v>327</v>
       </c>
       <c r="J29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K29" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -2579,10 +2579,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" t="s">
         <v>92</v>
-      </c>
-      <c r="C30" t="s">
-        <v>93</v>
       </c>
       <c r="D30" t="s">
         <v>13</v>
@@ -2591,19 +2591,19 @@
         <v>14</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -2611,10 +2611,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" t="s">
         <v>94</v>
-      </c>
-      <c r="C31" t="s">
-        <v>95</v>
       </c>
       <c r="D31" t="s">
         <v>13</v>
@@ -2623,19 +2623,19 @@
         <v>14</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -2643,10 +2643,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" t="s">
         <v>96</v>
-      </c>
-      <c r="C32" t="s">
-        <v>97</v>
       </c>
       <c r="D32" t="s">
         <v>13</v>
@@ -2655,19 +2655,19 @@
         <v>14</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -2675,10 +2675,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" t="s">
         <v>98</v>
-      </c>
-      <c r="C33" t="s">
-        <v>99</v>
       </c>
       <c r="D33" t="s">
         <v>13</v>
@@ -2687,19 +2687,19 @@
         <v>14</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -2707,10 +2707,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" t="s">
         <v>100</v>
-      </c>
-      <c r="C34" t="s">
-        <v>101</v>
       </c>
       <c r="D34" t="s">
         <v>13</v>
@@ -2719,19 +2719,19 @@
         <v>14</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -2739,10 +2739,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C35" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D35" t="s">
         <v>13</v>
@@ -2751,19 +2751,19 @@
         <v>14</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -2771,10 +2771,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C36" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D36" t="s">
         <v>13</v>
@@ -2783,19 +2783,19 @@
         <v>14</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -2803,10 +2803,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D37" t="s">
         <v>13</v>
@@ -2815,19 +2815,19 @@
         <v>14</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -2835,10 +2835,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38" t="s">
         <v>105</v>
-      </c>
-      <c r="C38" t="s">
-        <v>106</v>
       </c>
       <c r="D38" t="s">
         <v>13</v>
@@ -2847,19 +2847,19 @@
         <v>14</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -2867,10 +2867,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" t="s">
         <v>107</v>
-      </c>
-      <c r="C39" t="s">
-        <v>108</v>
       </c>
       <c r="D39" t="s">
         <v>13</v>
@@ -2879,19 +2879,19 @@
         <v>14</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -2899,10 +2899,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" t="s">
         <v>109</v>
-      </c>
-      <c r="C40" t="s">
-        <v>110</v>
       </c>
       <c r="D40" t="s">
         <v>13</v>
@@ -2911,19 +2911,19 @@
         <v>14</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -2931,31 +2931,31 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C41" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -2963,10 +2963,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42" t="s">
         <v>112</v>
-      </c>
-      <c r="C42" t="s">
-        <v>113</v>
       </c>
       <c r="D42" t="s">
         <v>13</v>
@@ -2975,19 +2975,19 @@
         <v>14</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -2995,31 +2995,31 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C43" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -3027,10 +3027,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C44" t="s">
         <v>115</v>
-      </c>
-      <c r="C44" t="s">
-        <v>116</v>
       </c>
       <c r="D44" t="s">
         <v>13</v>
@@ -3039,19 +3039,19 @@
         <v>14</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -3059,31 +3059,31 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C45" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -3091,10 +3091,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46" t="s">
         <v>118</v>
-      </c>
-      <c r="C46" t="s">
-        <v>119</v>
       </c>
       <c r="D46" t="s">
         <v>13</v>
@@ -3103,19 +3103,19 @@
         <v>14</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -3123,31 +3123,31 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C47" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -3155,10 +3155,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C48" t="s">
         <v>121</v>
-      </c>
-      <c r="C48" t="s">
-        <v>122</v>
       </c>
       <c r="D48" t="s">
         <v>13</v>
@@ -3167,19 +3167,19 @@
         <v>14</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -3187,31 +3187,31 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C49" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -3219,10 +3219,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C50" t="s">
         <v>124</v>
-      </c>
-      <c r="C50" t="s">
-        <v>125</v>
       </c>
       <c r="D50" t="s">
         <v>13</v>
@@ -3231,19 +3231,19 @@
         <v>14</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -3251,31 +3251,31 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C51" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -3283,10 +3283,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C52" t="s">
         <v>127</v>
-      </c>
-      <c r="C52" t="s">
-        <v>128</v>
       </c>
       <c r="D52" t="s">
         <v>13</v>
@@ -3295,19 +3295,19 @@
         <v>14</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -3315,31 +3315,31 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C53" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -3347,10 +3347,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C54" t="s">
         <v>130</v>
-      </c>
-      <c r="C54" t="s">
-        <v>131</v>
       </c>
       <c r="D54" t="s">
         <v>13</v>
@@ -3359,19 +3359,19 @@
         <v>14</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -3379,31 +3379,31 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C55" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D55" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -3411,10 +3411,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C56" t="s">
         <v>133</v>
-      </c>
-      <c r="C56" t="s">
-        <v>134</v>
       </c>
       <c r="D56" t="s">
         <v>13</v>
@@ -3423,19 +3423,19 @@
         <v>14</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -3443,31 +3443,31 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C57" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D57" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:11" s="1" customFormat="1">
@@ -3475,10 +3475,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C58" t="s">
         <v>136</v>
-      </c>
-      <c r="C58" t="s">
-        <v>137</v>
       </c>
       <c r="D58" t="s">
         <v>13</v>
@@ -3488,19 +3488,19 @@
       </c>
       <c r="F58" s="19"/>
       <c r="G58" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -3508,29 +3508,29 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C59" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D59" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I59" s="1"/>
       <c r="J59" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -3538,19 +3538,19 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C60" t="s">
+        <v>320</v>
+      </c>
+      <c r="D60" t="s">
+        <v>69</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F60" s="8" t="s">
         <v>139</v>
-      </c>
-      <c r="C60" t="s">
-        <v>322</v>
-      </c>
-      <c r="D60" t="s">
-        <v>70</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F60" s="8" t="s">
-        <v>140</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>21</v>
@@ -3571,10 +3571,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C61" t="s">
         <v>141</v>
-      </c>
-      <c r="C61" t="s">
-        <v>142</v>
       </c>
       <c r="D61" t="s">
         <v>13</v>
@@ -3583,19 +3583,19 @@
         <v>14</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -3603,31 +3603,31 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C62" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D62" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="63" spans="1:11">
@@ -3635,10 +3635,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C63" t="s">
         <v>144</v>
-      </c>
-      <c r="C63" t="s">
-        <v>145</v>
       </c>
       <c r="D63" t="s">
         <v>13</v>
@@ -3647,19 +3647,19 @@
         <v>14</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -3667,10 +3667,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C64" t="s">
         <v>146</v>
-      </c>
-      <c r="C64" t="s">
-        <v>147</v>
       </c>
       <c r="D64" t="s">
         <v>13</v>
@@ -3679,19 +3679,19 @@
         <v>14</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="65" spans="1:11">
@@ -3699,31 +3699,31 @@
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C65" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D65" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="66" spans="1:11">
@@ -3731,19 +3731,19 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C66" t="s">
+        <v>289</v>
+      </c>
+      <c r="D66" t="s">
+        <v>69</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F66" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="C66" t="s">
-        <v>291</v>
-      </c>
-      <c r="D66" t="s">
-        <v>70</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>150</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>21</v>
@@ -3764,19 +3764,19 @@
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C67" t="s">
+        <v>290</v>
+      </c>
+      <c r="D67" t="s">
+        <v>69</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F67" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C67" t="s">
-        <v>292</v>
-      </c>
-      <c r="D67" t="s">
-        <v>70</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>21</v>
@@ -3797,19 +3797,19 @@
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C68" t="s">
+        <v>291</v>
+      </c>
+      <c r="D68" t="s">
+        <v>69</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F68" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="C68" t="s">
-        <v>293</v>
-      </c>
-      <c r="D68" t="s">
-        <v>70</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>21</v>
@@ -3822,7 +3822,7 @@
         <v>16</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="69" spans="1:11" s="6" customFormat="1">
@@ -3830,32 +3830,32 @@
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C69" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F69" s="13"/>
       <c r="G69" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I69" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -3863,30 +3863,30 @@
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C70" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D70" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I70" s="2"/>
       <c r="J70" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -3894,30 +3894,30 @@
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C71" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D71" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F71" s="2"/>
       <c r="G71" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I71" s="2"/>
       <c r="J71" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="72" spans="1:11">
@@ -3925,30 +3925,30 @@
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C72" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F72" s="2"/>
       <c r="G72" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I72" s="2"/>
       <c r="J72" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="73" spans="1:11">
@@ -3956,30 +3956,30 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C73" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D73" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F73" s="2"/>
       <c r="G73" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I73" s="2"/>
       <c r="J73" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="74" spans="1:11" s="1" customFormat="1">
@@ -3987,30 +3987,30 @@
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C74" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D74" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F74" s="2"/>
       <c r="G74" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I74" s="2"/>
       <c r="J74" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="75" spans="1:11" s="1" customFormat="1">
@@ -4018,19 +4018,19 @@
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C75" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D75" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>21</v>
@@ -4051,30 +4051,30 @@
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C76" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D76" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F76" s="2"/>
       <c r="G76" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I76" s="2"/>
       <c r="J76" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="77" spans="1:11" s="1" customFormat="1">
@@ -4082,19 +4082,19 @@
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C77" t="s">
+        <v>300</v>
+      </c>
+      <c r="D77" t="s">
+        <v>69</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F77" s="19" t="s">
         <v>164</v>
-      </c>
-      <c r="C77" t="s">
-        <v>302</v>
-      </c>
-      <c r="D77" t="s">
-        <v>70</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F77" s="19" t="s">
-        <v>165</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>21</v>
@@ -4103,13 +4103,13 @@
         <v>21</v>
       </c>
       <c r="I77" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J77" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="78" spans="1:11">
@@ -4117,19 +4117,19 @@
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C78" t="s">
+        <v>301</v>
+      </c>
+      <c r="D78" t="s">
+        <v>69</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F78" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="C78" t="s">
-        <v>303</v>
-      </c>
-      <c r="D78" t="s">
-        <v>70</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>168</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>21</v>
@@ -4150,19 +4150,19 @@
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C79" t="s">
         <v>169</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
+        <v>69</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F79" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="D79" t="s">
-        <v>70</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>21</v>
@@ -4183,25 +4183,25 @@
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C80" t="s">
         <v>172</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D80" t="s">
+        <v>69</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F80" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D80" t="s">
-        <v>70</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F80" s="2" t="s">
+      <c r="G80" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H80" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="G80" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H80" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="I80" s="2"/>
       <c r="J80" s="2" t="s">
@@ -4216,25 +4216,25 @@
         <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C81" t="s">
         <v>176</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
+        <v>69</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F81" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D81" t="s">
-        <v>70</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F81" s="2" t="s">
+      <c r="G81" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H81" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H81" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="I81" s="2"/>
       <c r="J81" s="2" t="s">
@@ -4249,25 +4249,25 @@
         <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C82" t="s">
         <v>180</v>
       </c>
-      <c r="C82" t="s">
+      <c r="D82" t="s">
+        <v>69</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F82" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D82" t="s">
-        <v>70</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F82" s="2" t="s">
+      <c r="G82" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H82" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="G82" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H82" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="I82" s="2"/>
       <c r="J82" s="2" t="s">
@@ -4282,25 +4282,25 @@
         <v>82</v>
       </c>
       <c r="B83" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C83" t="s">
         <v>184</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
+        <v>69</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F83" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="D83" t="s">
-        <v>70</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F83" s="2" t="s">
+      <c r="G83" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H83" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H83" s="2" t="s">
-        <v>187</v>
       </c>
       <c r="I83" s="2"/>
       <c r="J83" s="2" t="s">
@@ -4315,25 +4315,25 @@
         <v>83</v>
       </c>
       <c r="B84" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C84" t="s">
         <v>188</v>
       </c>
-      <c r="C84" t="s">
+      <c r="D84" t="s">
+        <v>69</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F84" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D84" t="s">
-        <v>70</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F84" s="2" t="s">
+      <c r="G84" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H84" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="G84" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H84" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="I84" s="2"/>
       <c r="J84" s="2" t="s">
@@ -4348,25 +4348,25 @@
         <v>84</v>
       </c>
       <c r="B85" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C85" t="s">
         <v>192</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D85" t="s">
+        <v>69</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F85" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="D85" t="s">
-        <v>70</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F85" s="2" t="s">
+      <c r="G85" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H85" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H85" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="I85" s="2"/>
       <c r="J85" s="2" t="s">
@@ -4381,25 +4381,25 @@
         <v>85</v>
       </c>
       <c r="B86" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C86" t="s">
         <v>196</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
+        <v>69</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F86" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D86" t="s">
-        <v>70</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F86" s="2" t="s">
+      <c r="G86" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H86" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H86" s="2" t="s">
-        <v>199</v>
       </c>
       <c r="I86" s="2"/>
       <c r="J86" s="2" t="s">
@@ -4414,25 +4414,25 @@
         <v>86</v>
       </c>
       <c r="B87" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C87" t="s">
         <v>200</v>
       </c>
-      <c r="C87" t="s">
+      <c r="D87" t="s">
+        <v>69</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F87" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="D87" t="s">
-        <v>70</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F87" s="2" t="s">
+      <c r="G87" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H87" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H87" s="2" t="s">
-        <v>203</v>
       </c>
       <c r="I87" s="2"/>
       <c r="J87" s="2" t="s">
@@ -4447,30 +4447,30 @@
         <v>87</v>
       </c>
       <c r="B88" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C88" t="s">
         <v>204</v>
       </c>
-      <c r="C88" t="s">
-        <v>205</v>
-      </c>
       <c r="D88" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F88" s="2"/>
       <c r="G88" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I88" s="2"/>
       <c r="J88" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="89" spans="1:11">
@@ -4478,30 +4478,30 @@
         <v>88</v>
       </c>
       <c r="B89" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C89" t="s">
         <v>206</v>
       </c>
-      <c r="C89" t="s">
-        <v>207</v>
-      </c>
       <c r="D89" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F89" s="2"/>
       <c r="G89" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I89" s="2"/>
       <c r="J89" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="90" spans="1:11">
@@ -4509,30 +4509,30 @@
         <v>89</v>
       </c>
       <c r="B90" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C90" t="s">
         <v>208</v>
       </c>
-      <c r="C90" t="s">
-        <v>209</v>
-      </c>
       <c r="D90" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F90" s="2"/>
       <c r="G90" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I90" s="2"/>
       <c r="J90" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="91" spans="1:11">
@@ -4540,25 +4540,25 @@
         <v>90</v>
       </c>
       <c r="B91" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C91" t="s">
         <v>210</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
+        <v>69</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F91" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D91" t="s">
-        <v>70</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F91" s="2" t="s">
+      <c r="G91" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H91" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="G91" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H91" s="2" t="s">
-        <v>213</v>
       </c>
       <c r="I91" s="2"/>
       <c r="J91" s="2" t="s">
@@ -4573,25 +4573,25 @@
         <v>91</v>
       </c>
       <c r="B92" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C92" t="s">
         <v>214</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D92" t="s">
+        <v>69</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F92" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="D92" t="s">
-        <v>70</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F92" s="2" t="s">
+      <c r="G92" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H92" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="G92" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H92" s="2" t="s">
-        <v>217</v>
       </c>
       <c r="I92" s="2"/>
       <c r="J92" s="2" t="s">
@@ -4606,19 +4606,19 @@
         <v>92</v>
       </c>
       <c r="B93" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C93" t="s">
         <v>218</v>
       </c>
-      <c r="C93" t="s">
-        <v>219</v>
-      </c>
       <c r="D93" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>21</v>
@@ -4627,7 +4627,7 @@
         <v>21</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J93" s="2" t="s">
         <v>16</v>
@@ -4641,19 +4641,19 @@
         <v>93</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C94" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D94" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>21</v>
@@ -4662,7 +4662,7 @@
         <v>21</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J94" s="2" t="s">
         <v>16</v>
@@ -4676,19 +4676,19 @@
         <v>94</v>
       </c>
       <c r="B95" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C95" t="s">
+        <v>322</v>
+      </c>
+      <c r="D95" t="s">
+        <v>69</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F95" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="C95" t="s">
-        <v>324</v>
-      </c>
-      <c r="D95" t="s">
-        <v>70</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="G95" s="2" t="s">
         <v>21</v>
@@ -4709,25 +4709,25 @@
         <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C96" t="s">
+        <v>323</v>
+      </c>
+      <c r="D96" t="s">
+        <v>69</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F96" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="C96" t="s">
-        <v>325</v>
-      </c>
-      <c r="D96" t="s">
-        <v>70</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F96" s="3" t="s">
+      <c r="G96" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H96" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="G96" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H96" s="2" t="s">
-        <v>226</v>
       </c>
       <c r="I96" s="2"/>
       <c r="J96" s="2" t="s">
@@ -4742,32 +4742,32 @@
         <v>96</v>
       </c>
       <c r="B97" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C97" t="s">
         <v>227</v>
       </c>
-      <c r="C97" t="s">
+      <c r="D97" t="s">
+        <v>69</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F97" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="D97" t="s">
-        <v>70</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F97" s="3" t="s">
+      <c r="G97" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H97" s="3" t="s">
         <v>229</v>
-      </c>
-      <c r="G97" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H97" s="3" t="s">
-        <v>230</v>
       </c>
       <c r="I97" s="2"/>
       <c r="J97" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K97" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="98" spans="1:11" ht="75">
@@ -4775,32 +4775,32 @@
         <v>97</v>
       </c>
       <c r="B98" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C98" t="s">
+        <v>303</v>
+      </c>
+      <c r="D98" t="s">
+        <v>69</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F98" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="C98" t="s">
-        <v>305</v>
-      </c>
-      <c r="D98" t="s">
-        <v>70</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F98" s="3" t="s">
+      <c r="G98" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H98" s="3" t="s">
         <v>232</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H98" s="3" t="s">
-        <v>233</v>
       </c>
       <c r="I98" s="2"/>
       <c r="J98" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="99" spans="1:11" ht="60">
@@ -4808,32 +4808,32 @@
         <v>98</v>
       </c>
       <c r="B99" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C99" t="s">
+        <v>304</v>
+      </c>
+      <c r="D99" t="s">
+        <v>69</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F99" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="C99" t="s">
-        <v>306</v>
-      </c>
-      <c r="D99" t="s">
-        <v>70</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F99" s="3" t="s">
+      <c r="G99" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H99" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="G99" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H99" s="3" t="s">
-        <v>236</v>
       </c>
       <c r="I99" s="2"/>
       <c r="J99" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="100" spans="1:11" ht="30">
@@ -4841,32 +4841,32 @@
         <v>99</v>
       </c>
       <c r="B100" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C100" t="s">
+        <v>305</v>
+      </c>
+      <c r="D100" t="s">
+        <v>69</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F100" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="C100" t="s">
-        <v>307</v>
-      </c>
-      <c r="D100" t="s">
-        <v>70</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F100" s="3" t="s">
+      <c r="G100" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H100" s="3" t="s">
         <v>238</v>
-      </c>
-      <c r="G100" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H100" s="3" t="s">
-        <v>239</v>
       </c>
       <c r="I100" s="2"/>
       <c r="J100" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K100" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="101" spans="1:11">
@@ -4874,30 +4874,30 @@
         <v>100</v>
       </c>
       <c r="B101" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C101" t="s">
         <v>240</v>
       </c>
-      <c r="C101" t="s">
-        <v>241</v>
-      </c>
       <c r="D101" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F101" s="2"/>
       <c r="G101" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I101" s="2"/>
       <c r="J101" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K101" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="102" spans="1:11" ht="75">
@@ -4905,32 +4905,32 @@
         <v>101</v>
       </c>
       <c r="B102" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C102" t="s">
         <v>242</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D102" t="s">
+        <v>69</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F102" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="D102" t="s">
-        <v>70</v>
-      </c>
-      <c r="E102" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F102" s="3" t="s">
+      <c r="G102" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H102" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="G102" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H102" s="3" t="s">
-        <v>245</v>
       </c>
       <c r="I102" s="2"/>
       <c r="J102" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="103" spans="1:11">
@@ -4938,30 +4938,30 @@
         <v>102</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C103" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D103" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F103" s="2"/>
       <c r="G103" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I103" s="2"/>
       <c r="J103" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K103" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="104" spans="1:11" ht="60">
@@ -4969,32 +4969,32 @@
         <v>103</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C104" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D104" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F104" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H104" s="3" t="s">
         <v>263</v>
-      </c>
-      <c r="G104" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H104" s="3" t="s">
-        <v>264</v>
       </c>
       <c r="I104" s="2"/>
       <c r="J104" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K104" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="105" spans="1:11" ht="30">
@@ -5002,32 +5002,32 @@
         <v>104</v>
       </c>
       <c r="B105" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C105" t="s">
         <v>248</v>
       </c>
-      <c r="C105" t="s">
-        <v>249</v>
-      </c>
       <c r="D105" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F105" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H105" s="3" t="s">
         <v>265</v>
-      </c>
-      <c r="G105" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H105" s="3" t="s">
-        <v>266</v>
       </c>
       <c r="I105" s="2"/>
       <c r="J105" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K105" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="106" spans="1:11" ht="60">
@@ -5035,32 +5035,32 @@
         <v>105</v>
       </c>
       <c r="B106" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C106" t="s">
         <v>250</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D106" t="s">
+        <v>69</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F106" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="D106" t="s">
-        <v>70</v>
-      </c>
-      <c r="E106" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F106" s="3" t="s">
+      <c r="G106" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H106" s="3" t="s">
         <v>252</v>
-      </c>
-      <c r="G106" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H106" s="3" t="s">
-        <v>253</v>
       </c>
       <c r="I106" s="2"/>
       <c r="J106" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K106" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="107" spans="1:11">
@@ -5068,30 +5068,30 @@
         <v>106</v>
       </c>
       <c r="B107" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C107" t="s">
         <v>254</v>
       </c>
-      <c r="C107" t="s">
-        <v>255</v>
-      </c>
       <c r="D107" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F107" s="2"/>
       <c r="G107" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I107" s="2"/>
       <c r="J107" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K107" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="108" spans="1:11">
@@ -5099,19 +5099,19 @@
         <v>107</v>
       </c>
       <c r="B108" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C108" t="s">
         <v>256</v>
       </c>
-      <c r="C108" t="s">
+      <c r="D108" t="s">
+        <v>69</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F108" s="2" t="s">
         <v>257</v>
-      </c>
-      <c r="D108" t="s">
-        <v>70</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F108" s="2" t="s">
-        <v>258</v>
       </c>
       <c r="G108" s="2" t="s">
         <v>21</v>
@@ -5132,10 +5132,10 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
+        <v>258</v>
+      </c>
+      <c r="C109" t="s">
         <v>259</v>
-      </c>
-      <c r="C109" t="s">
-        <v>260</v>
       </c>
       <c r="D109" t="s">
         <v>13</v>
@@ -5144,16 +5144,16 @@
         <v>14</v>
       </c>
       <c r="F109" s="25" t="s">
+        <v>260</v>
+      </c>
+      <c r="G109" s="26" t="s">
         <v>261</v>
-      </c>
-      <c r="G109" s="26" t="s">
-        <v>262</v>
       </c>
       <c r="H109">
         <v>1</v>
       </c>
       <c r="I109" s="27" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J109" s="11" t="s">
         <v>16</v>
@@ -5236,6 +5236,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
@@ -5247,7 +5256,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -5488,16 +5497,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07CD54F7-7682-4260-A57C-9131D22DC2E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B65EFA2E-A807-485E-9383-5A8846A1595A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -5508,7 +5516,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B924E26-FD9D-4578-A9DC-389C0AAF7136}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5525,12 +5533,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07CD54F7-7682-4260-A57C-9131D22DC2E8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>